<commit_message>
fix: fix celery for receiving traffic; add load_app func
</commit_message>
<xml_diff>
--- a/algorithm-side-interfaces/algorithm/data/test.xlsx
+++ b/algorithm-side-interfaces/algorithm/data/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,7 +532,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-03-01 14:57:10</t>
+          <t>2025-03-06 08:54:05</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-03-01 14:57:10</t>
+          <t>2025-03-06 08:54:05</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -627,7 +627,7 @@
         <v>200</v>
       </c>
       <c r="M3" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="N3" t="n">
         <v>1</v>
@@ -644,17 +644,17 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-03-01 14:57:10</t>
+          <t>2025-03-06 08:54:05</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -664,12 +664,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
+          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>/api/v1/resource/16</t>
+          <t>/api/v1/memo/21</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -705,17 +705,17 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-03-01 14:57:10</t>
+          <t>2025-03-06 08:54:05</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -725,12 +725,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>/api/v1/memo/21</t>
+          <t>/api/v1/resource/16</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -749,18 +749,140 @@
         <v>200</v>
       </c>
       <c r="M5" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-03-06 08:54:05</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>DELETE</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>/api/v1/memo/21</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>200</v>
+      </c>
+      <c r="M6" t="n">
         <v>0.003</v>
       </c>
-      <c r="N5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="b">
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-03-06 08:54:05</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>DELETE</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>/api/v1/memo/21</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" t="n">
+        <v>5</v>
+      </c>
+      <c r="L7" t="n">
+        <v>200</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: add user setting sample APi seqs
</commit_message>
<xml_diff>
--- a/algorithm-side-interfaces/algorithm/data/test.xlsx
+++ b/algorithm-side-interfaces/algorithm/data/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,7 +532,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-03-06 08:54:05</t>
+          <t>2025-03-06 12:03:12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -542,12 +542,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+          <t>http://47.97.114.24:5230/api/v1/resource/16</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>/api/v1/memo/21</t>
+          <t>/api/v1/resource/16</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -566,10 +566,10 @@
         <v>200</v>
       </c>
       <c r="M2" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="Q2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -586,14 +586,14 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-03-06 08:54:05</t>
+          <t>2025-03-06 12:03:12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -603,12 +603,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
+          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>/api/v1/resource/16</t>
+          <t>/api/v1/memo/21</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -633,10 +633,10 @@
         <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="b">
         <v>0</v>
@@ -654,7 +654,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-03-06 08:54:05</t>
+          <t>2025-03-06 12:03:12</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -688,19 +688,19 @@
         <v>200</v>
       </c>
       <c r="M4" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -715,7 +715,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-03-06 08:54:05</t>
+          <t>2025-03-06 12:03:12</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -725,12 +725,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
+          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>/api/v1/resource/16</t>
+          <t>/api/v1/memo/21</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -749,34 +749,34 @@
         <v>200</v>
       </c>
       <c r="M5" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-03-06 08:54:05</t>
+          <t>2025-03-06 12:03:12</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -786,12 +786,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>/api/v1/memo/21</t>
+          <t>/api/v1/resource/16</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -810,10 +810,10 @@
         <v>200</v>
       </c>
       <c r="M6" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
@@ -822,68 +822,7 @@
         <v>1</v>
       </c>
       <c r="Q6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>7</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2025-03-06 08:54:05</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>DELETE</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>/api/v1/memo/21</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" t="n">
-        <v>5</v>
-      </c>
-      <c r="L7" t="n">
-        <v>200</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="N7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" t="n">
-        <v>1</v>
-      </c>
-      <c r="P7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update backend interfaces
</commit_message>
<xml_diff>
--- a/algorithm-side-interfaces/algorithm/data/test.xlsx
+++ b/algorithm-side-interfaces/algorithm/data/test.xlsx
@@ -532,7 +532,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-03-06 12:03:12</t>
+          <t>2025-03-09 06:05:12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://47.97.114.24:5230/api/v1/resource/16</t>
+          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -566,10 +566,10 @@
         <v>200</v>
       </c>
       <c r="M2" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="Q2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -586,14 +586,14 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-03-06 12:03:12</t>
+          <t>2025-03-09 06:05:12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -603,12 +603,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>/api/v1/memo/21</t>
+          <t>/api/v1/resource/16</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -633,10 +633,10 @@
         <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="b">
         <v>0</v>
@@ -654,7 +654,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-03-06 12:03:12</t>
+          <t>2025-03-09 06:05:12</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -688,19 +688,19 @@
         <v>200</v>
       </c>
       <c r="M4" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -715,7 +715,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-03-06 12:03:12</t>
+          <t>2025-03-09 06:05:12</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -725,12 +725,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+          <t>http://47.97.114.24:5230/api/v1/resource/16</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>/api/v1/memo/21</t>
+          <t>/api/v1/resource/16</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -752,16 +752,16 @@
         <v>0.003</v>
       </c>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -776,7 +776,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-03-06 12:03:12</t>
+          <t>2025-03-09 06:05:12</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -786,12 +786,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
+          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>/api/v1/resource/16</t>
+          <t>/api/v1/memo/21</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -810,19 +810,19 @@
         <v>200</v>
       </c>
       <c r="M6" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix backend and algorithm-side bugs
</commit_message>
<xml_diff>
--- a/algorithm-side-interfaces/algorithm/data/test.xlsx
+++ b/algorithm-side-interfaces/algorithm/data/test.xlsx
@@ -532,22 +532,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-03-10 09:09:54</t>
+          <t>2025-03-15 13:19:21</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
+          <t>http://49.234.6.241:5230/memos.api.v1.UserService/CreateUserAccessToken</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>/api/v1/resource/16</t>
+          <t>/memos.api.v1.UserService/CreateUserAccessToken</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -566,10 +566,10 @@
         <v>200</v>
       </c>
       <c r="M2" t="n">
-        <v>0.007</v>
+        <v>0.004</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="Q2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -593,22 +593,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-03-10 09:09:54</t>
+          <t>2025-03-15 13:19:21</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+          <t>http://49.234.6.241:5230/memos.api.v1.MemoService/CreateMemo</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>/api/v1/memo/21</t>
+          <t>/memos.api.v1.MemoService/CreateMemo</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -627,19 +627,19 @@
         <v>200</v>
       </c>
       <c r="M3" t="n">
-        <v>0.006</v>
+        <v>0.003</v>
       </c>
       <c r="N3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -654,22 +654,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-03-10 09:09:54</t>
+          <t>2025-03-15 13:19:21</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://47.97.114.24:5230/api/v1/resource/16</t>
+          <t>http://49.234.6.241:5230/memos.api.v1.UserService/CreateUserAccessToken</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>/api/v1/resource/16</t>
+          <t>/memos.api.v1.UserService/CreateUserAccessToken</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -688,7 +688,7 @@
         <v>200</v>
       </c>
       <c r="M4" t="n">
-        <v>0.006</v>
+        <v>0.002</v>
       </c>
       <c r="N4" t="n">
         <v>1</v>
@@ -715,22 +715,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-03-10 09:09:54</t>
+          <t>2025-03-15 13:19:21</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+          <t>http://49.234.6.241:5230/memos.api.v1.MemoService/CreateMemo</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>/api/v1/memo/21</t>
+          <t>/memos.api.v1.MemoService/CreateMemo</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -749,7 +749,7 @@
         <v>200</v>
       </c>
       <c r="M5" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="N5" t="n">
         <v>1</v>
@@ -776,22 +776,22 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-03-10 09:09:54</t>
+          <t>2025-03-15 13:19:21</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
+          <t>http://49.234.6.241:5230/memos.api.v1.UserService/CreateUserAccessToken</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>/api/v1/resource/16</t>
+          <t>/memos.api.v1.UserService/CreateUserAccessToken</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -837,22 +837,22 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-03-10 09:09:54</t>
+          <t>2025-03-15 13:19:21</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+          <t>http://49.234.6.241:5230/memos.api.v1.MemoService/CreateMemo</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>/api/v1/memo/21</t>
+          <t>/memos.api.v1.MemoService/CreateMemo</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -871,7 +871,7 @@
         <v>200</v>
       </c>
       <c r="M7" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -898,22 +898,22 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-03-10 09:09:54</t>
+          <t>2025-03-15 13:19:21</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/resource/16</t>
+          <t>http://49.234.6.241:5230/memos.api.v1.UserService/CreateUserAccessToken</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>/api/v1/resource/16</t>
+          <t>/memos.api.v1.UserService/CreateUserAccessToken</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -932,10 +932,10 @@
         <v>200</v>
       </c>
       <c r="M8" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="Q8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -959,22 +959,22 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-03-10 09:09:54</t>
+          <t>2025-03-15 13:19:21</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>http://49.234.6.241:5230/api/v1/memo/21</t>
+          <t>http://49.234.6.241:5230/memos.api.v1.MemoService/CreateMemo</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>/api/v1/memo/21</t>
+          <t>/memos.api.v1.MemoService/CreateMemo</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -993,19 +993,19 @@
         <v>200</v>
       </c>
       <c r="M9" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>